<commit_message>
update bg with full easq data
</commit_message>
<xml_diff>
--- a/bg_missing_counts.xlsx
+++ b/bg_missing_counts.xlsx
@@ -994,17 +994,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C2">
         <v>921</v>
       </c>
       <c r="D2">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E2">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F2">
         <v>1761</v>
@@ -1021,23 +1021,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C3">
         <v>921</v>
       </c>
       <c r="D3">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E3">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="F3">
         <v>1761</v>
       </c>
       <c r="G3">
-        <v>0.569</v>
+        <v>0.5659999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -1048,23 +1048,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C4">
         <v>921</v>
       </c>
       <c r="D4">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="F4">
         <v>1761</v>
       </c>
       <c r="G4">
-        <v>0.5679999999999999</v>
+        <v>0.5659999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -1075,23 +1075,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C5">
         <v>921</v>
       </c>
       <c r="D5">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E5">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="F5">
         <v>1761</v>
       </c>
       <c r="G5">
-        <v>0.5679999999999999</v>
+        <v>0.5659999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -1156,23 +1156,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C8">
         <v>919</v>
       </c>
       <c r="D8">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="F8">
         <v>1761</v>
       </c>
       <c r="G8">
-        <v>0.5649999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -1183,23 +1183,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C9">
         <v>919</v>
       </c>
       <c r="D9">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E9">
-        <v>1000</v>
+        <v>994</v>
       </c>
       <c r="F9">
         <v>1761</v>
       </c>
       <c r="G9">
-        <v>0.5679999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1210,23 +1210,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C10">
         <v>919</v>
       </c>
       <c r="D10">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E10">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="F10">
         <v>1761</v>
       </c>
       <c r="G10">
-        <v>0.5669999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1237,23 +1237,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C11">
         <v>919</v>
       </c>
       <c r="D11">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E11">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="F11">
         <v>1761</v>
       </c>
       <c r="G11">
-        <v>0.5669999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="12">
@@ -1318,17 +1318,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C14">
         <v>918</v>
       </c>
       <c r="D14">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E14">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F14">
         <v>1761</v>
@@ -1345,23 +1345,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C15">
         <v>918</v>
       </c>
       <c r="D15">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E15">
-        <v>999</v>
+        <v>993</v>
       </c>
       <c r="F15">
         <v>1761</v>
       </c>
       <c r="G15">
-        <v>0.5669999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="16">
@@ -1372,23 +1372,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C16">
         <v>918</v>
       </c>
       <c r="D16">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E16">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="F16">
         <v>1761</v>
       </c>
       <c r="G16">
-        <v>0.5659999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="17">
@@ -1399,23 +1399,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C17">
         <v>918</v>
       </c>
       <c r="D17">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E17">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="F17">
         <v>1761</v>
       </c>
       <c r="G17">
-        <v>0.5659999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="18">
@@ -1480,23 +1480,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C20">
         <v>727</v>
       </c>
       <c r="D20">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E20">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F20">
         <v>1761</v>
       </c>
       <c r="G20">
-        <v>0.463</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="21">
@@ -1507,23 +1507,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C21">
         <v>727</v>
       </c>
       <c r="D21">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E21">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F21">
         <v>1761</v>
       </c>
       <c r="G21">
-        <v>0.464</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="22">
@@ -1534,23 +1534,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C22">
         <v>727</v>
       </c>
       <c r="D22">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E22">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="F22">
         <v>1761</v>
       </c>
       <c r="G22">
-        <v>0.465</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="23">
@@ -1561,23 +1561,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C23">
         <v>727</v>
       </c>
       <c r="D23">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E23">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F23">
         <v>1761</v>
       </c>
       <c r="G23">
-        <v>0.464</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="24">
@@ -1642,23 +1642,23 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C26">
         <v>727</v>
       </c>
       <c r="D26">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E26">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F26">
         <v>1761</v>
       </c>
       <c r="G26">
-        <v>0.463</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="27">
@@ -1669,23 +1669,23 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C27">
         <v>727</v>
       </c>
       <c r="D27">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E27">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F27">
         <v>1761</v>
       </c>
       <c r="G27">
-        <v>0.464</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="28">
@@ -1696,23 +1696,23 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C28">
         <v>727</v>
       </c>
       <c r="D28">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E28">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="F28">
         <v>1761</v>
       </c>
       <c r="G28">
-        <v>0.465</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="29">
@@ -1723,23 +1723,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C29">
         <v>727</v>
       </c>
       <c r="D29">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E29">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F29">
         <v>1761</v>
       </c>
       <c r="G29">
-        <v>0.464</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="30">
@@ -1804,23 +1804,23 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C32">
         <v>333</v>
       </c>
       <c r="D32">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E32">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F32">
         <v>1761</v>
       </c>
       <c r="G32">
-        <v>0.24</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="33">
@@ -1831,23 +1831,23 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C33">
         <v>333</v>
       </c>
       <c r="D33">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E33">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="F33">
         <v>1761</v>
       </c>
       <c r="G33">
-        <v>0.245</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="34">
@@ -1858,23 +1858,23 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C34">
         <v>333</v>
       </c>
       <c r="D34">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E34">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="F34">
         <v>1761</v>
       </c>
       <c r="G34">
-        <v>0.244</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="35">
@@ -1885,23 +1885,23 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C35">
         <v>333</v>
       </c>
       <c r="D35">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E35">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F35">
         <v>1761</v>
       </c>
       <c r="G35">
-        <v>0.24</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="36">
@@ -1966,23 +1966,23 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C38">
         <v>334</v>
       </c>
       <c r="D38">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E38">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F38">
         <v>1761</v>
       </c>
       <c r="G38">
-        <v>0.241</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="39">
@@ -1993,23 +1993,23 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C39">
         <v>334</v>
       </c>
       <c r="D39">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E39">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="F39">
         <v>1761</v>
       </c>
       <c r="G39">
-        <v>0.246</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="40">
@@ -2020,23 +2020,23 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C40">
         <v>334</v>
       </c>
       <c r="D40">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E40">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="F40">
         <v>1761</v>
       </c>
       <c r="G40">
-        <v>0.244</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="41">
@@ -2047,23 +2047,23 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C41">
         <v>334</v>
       </c>
       <c r="D41">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E41">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F41">
         <v>1761</v>
       </c>
       <c r="G41">
-        <v>0.241</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="42">
@@ -2128,23 +2128,23 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C44">
         <v>333</v>
       </c>
       <c r="D44">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E44">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F44">
         <v>1761</v>
       </c>
       <c r="G44">
-        <v>0.24</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="45">
@@ -2155,23 +2155,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C45">
         <v>333</v>
       </c>
       <c r="D45">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E45">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="F45">
         <v>1761</v>
       </c>
       <c r="G45">
-        <v>0.245</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="46">
@@ -2182,23 +2182,23 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C46">
         <v>333</v>
       </c>
       <c r="D46">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E46">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="F46">
         <v>1761</v>
       </c>
       <c r="G46">
-        <v>0.244</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="47">
@@ -2209,23 +2209,23 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C47">
         <v>333</v>
       </c>
       <c r="D47">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E47">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F47">
         <v>1761</v>
       </c>
       <c r="G47">
-        <v>0.24</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="48">
@@ -2290,23 +2290,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C50">
         <v>374</v>
       </c>
       <c r="D50">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E50">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="F50">
         <v>1761</v>
       </c>
       <c r="G50">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="51">
@@ -2317,23 +2317,23 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C51">
         <v>374</v>
       </c>
       <c r="D51">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E51">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="F51">
         <v>1761</v>
       </c>
       <c r="G51">
-        <v>0.263</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="52">
@@ -2344,23 +2344,23 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C52">
         <v>374</v>
       </c>
       <c r="D52">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E52">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="F52">
         <v>1761</v>
       </c>
       <c r="G52">
-        <v>0.263</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="53">
@@ -2371,23 +2371,23 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C53">
         <v>374</v>
       </c>
       <c r="D53">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E53">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="F53">
         <v>1761</v>
       </c>
       <c r="G53">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="54">
@@ -2452,23 +2452,23 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C56">
         <v>374</v>
       </c>
       <c r="D56">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E56">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="F56">
         <v>1761</v>
       </c>
       <c r="G56">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="57">
@@ -2479,23 +2479,23 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C57">
         <v>374</v>
       </c>
       <c r="D57">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E57">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="F57">
         <v>1761</v>
       </c>
       <c r="G57">
-        <v>0.263</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="58">
@@ -2506,23 +2506,23 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C58">
         <v>374</v>
       </c>
       <c r="D58">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E58">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="F58">
         <v>1761</v>
       </c>
       <c r="G58">
-        <v>0.263</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="59">
@@ -2533,23 +2533,23 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C59">
         <v>374</v>
       </c>
       <c r="D59">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E59">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="F59">
         <v>1761</v>
       </c>
       <c r="G59">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="60">
@@ -2664,23 +2664,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>z_age2mo_personal_no4</t>
+          <t>z_age2mo_personal_all</t>
         </is>
       </c>
       <c r="C2">
         <v>335</v>
       </c>
       <c r="D2">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E2">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F2">
         <v>1761</v>
       </c>
       <c r="G2">
-        <v>0.241</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3">
@@ -2691,23 +2691,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>z_age2mo_motor_no4</t>
+          <t>z_age2mo_motor_all</t>
         </is>
       </c>
       <c r="C3">
         <v>335</v>
       </c>
       <c r="D3">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E3">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="F3">
         <v>1761</v>
       </c>
       <c r="G3">
-        <v>0.246</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="4">
@@ -2718,23 +2718,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>z_age2mo_combined_no4</t>
+          <t>z_age2mo_combined_all</t>
         </is>
       </c>
       <c r="C4">
         <v>335</v>
       </c>
       <c r="D4">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E4">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="F4">
         <v>1761</v>
       </c>
       <c r="G4">
-        <v>0.245</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="5">
@@ -2745,23 +2745,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>z_age2mo_com_no4</t>
+          <t>z_age2mo_com_all</t>
         </is>
       </c>
       <c r="C5">
         <v>335</v>
       </c>
       <c r="D5">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E5">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F5">
         <v>1761</v>
       </c>
       <c r="G5">
-        <v>0.241</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
update tables with ln(lac/mann)
</commit_message>
<xml_diff>
--- a/bg_missing_counts.xlsx
+++ b/bg_missing_counts.xlsx
@@ -723,7 +723,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -750,7 +750,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -777,7 +777,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -831,7 +831,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -858,7 +858,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -885,7 +885,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -912,7 +912,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1475,7 +1475,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1502,7 +1502,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1529,7 +1529,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1556,7 +1556,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1583,7 +1583,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1610,7 +1610,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>L_conc_t1</t>
+          <t>ln_L_conc_t1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1637,7 +1637,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1664,7 +1664,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1691,7 +1691,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1745,7 +1745,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1772,7 +1772,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>M_conc_t1</t>
+          <t>ln_M_conc_t1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">

</xml_diff>

<commit_message>
use log trans exp vars
</commit_message>
<xml_diff>
--- a/bg_missing_counts.xlsx
+++ b/bg_missing_counts.xlsx
@@ -399,7 +399,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -426,7 +426,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -453,7 +453,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -534,7 +534,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -561,7 +561,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -615,7 +615,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -642,7 +642,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -669,7 +669,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -696,7 +696,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -989,7 +989,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1016,7 +1016,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1043,7 +1043,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1070,7 +1070,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1097,7 +1097,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1124,7 +1124,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>aat1</t>
+          <t>ln_aat1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1151,7 +1151,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1205,7 +1205,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1232,7 +1232,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1259,7 +1259,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1286,7 +1286,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>mpo1</t>
+          <t>ln_mpo1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1313,7 +1313,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1340,7 +1340,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1367,7 +1367,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1394,7 +1394,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1421,7 +1421,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>neo1</t>
+          <t>ln_neo1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1799,7 +1799,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>ln_aat2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1826,7 +1826,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>ln_aat2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1853,7 +1853,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>ln_aat2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1880,7 +1880,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>ln_aat2</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1907,7 +1907,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>ln_aat2</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1934,7 +1934,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>aat2</t>
+          <t>ln_aat2</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1961,7 +1961,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>ln_mpo2</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>ln_mpo2</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2015,7 +2015,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>ln_mpo2</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2042,7 +2042,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>ln_mpo2</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2069,7 +2069,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>ln_mpo2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mpo2</t>
+          <t>ln_mpo2</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2123,7 +2123,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>ln_neo2</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2150,7 +2150,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>ln_neo2</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2177,7 +2177,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>ln_neo2</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>ln_neo2</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2231,7 +2231,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>ln_neo2</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>neo2</t>
+          <t>ln_neo2</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">

</xml_diff>